<commit_message>
Add more controller data
</commit_message>
<xml_diff>
--- a/data/controllers/controller_data.xlsx
+++ b/data/controllers/controller_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/data/controllers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C4180-23E0-D347-B4B0-F8123A674553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66251BCF-8C12-7B40-A861-D7582CFAF6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{2F87124F-FADD-1C4B-8E1F-F5E2F237BAFB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="134">
   <si>
     <t>No</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>*nominal: speed at peak power</t>
   </si>
   <si>
     <t>JM1S</t>
@@ -391,12 +388,6 @@
     <t>UHV-28S</t>
   </si>
   <si>
-    <t>w/ cables</t>
-  </si>
-  <si>
-    <t>w/o cables</t>
-  </si>
-  <si>
     <t>Embention</t>
   </si>
   <si>
@@ -410,6 +401,45 @@
   </si>
   <si>
     <t>https://www.embention.com/</t>
+  </si>
+  <si>
+    <t>P [kW]</t>
+  </si>
+  <si>
+    <t>W [kg]</t>
+  </si>
+  <si>
+    <t>BRUSA HyPower</t>
+  </si>
+  <si>
+    <t>https://www.brusahypower.com/products/</t>
+  </si>
+  <si>
+    <t>DMC514</t>
+  </si>
+  <si>
+    <t>DMC524</t>
+  </si>
+  <si>
+    <t>DMC534</t>
+  </si>
+  <si>
+    <t>DMC544</t>
+  </si>
+  <si>
+    <t>BDC546</t>
+  </si>
+  <si>
+    <t>BDC668</t>
+  </si>
+  <si>
+    <t>BorgWarner</t>
+  </si>
+  <si>
+    <t>https://www.borgwarner.com/</t>
+  </si>
+  <si>
+    <t>Gen4 Size 8</t>
   </si>
 </sst>
 </file>
@@ -671,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -733,22 +763,19 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -758,7 +785,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -770,23 +821,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -794,22 +836,31 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -830,65 +881,68 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1018,9 +1072,16 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.10582552857847045"/>
+                  <c:y val="0.1939745290111369"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1053,29 +1114,41 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$7:$G$13</c:f>
+              <c:f>Sheet1!$G$10:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
@@ -1083,29 +1156,41 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$13</c:f>
+              <c:f>Sheet1!$E$10:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.74</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2799999999999998</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>1.8</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>6.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -1115,6 +1200,283 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-29E9-0641-A0EC-F21814FF4DA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>from_paper</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.16957099487328783"/>
+                  <c:y val="9.2901358802534913E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$18:$U$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$18:$T$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>1.1030150753768846</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3567839195979903</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6105527638190957</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1180904522613062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3718592964824126</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6256281407035171</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8793969849246235</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.13316582914573</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.386934673366834</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.640703517587941</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.894472361809045</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.148241206030153</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.40201005025126</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.655778894472366</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.909547738693469</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.163316582914575</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.417085427135682</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.670854271356788</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.924623115577894</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.178391959798997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>27.432160804020103</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>28.68592964824121</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>29.939698492462316</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31.193467336683423</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>32.447236180904525</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33.701005025125632</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34.954773869346738</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36.208542713567844</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37.462311557788951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0FC9-5244-A6DF-E79D343E80E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10431,13 +10793,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>128567</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>196301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>545629</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>85921</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11016,10 +11378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6965AA0C-F6DC-7C4E-924A-27408B62696D}">
-  <dimension ref="B2:N13"/>
+  <dimension ref="B2:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11031,64 +11393,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="5" spans="2:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="I5" s="24"/>
-      <c r="J5" s="72" t="s">
-        <v>122</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>20</v>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="6" t="s">
         <v>4</v>
       </c>
@@ -11101,21 +11463,19 @@
       <c r="I6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="73"/>
-      <c r="K6" s="24"/>
-      <c r="N6" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="J6" s="34"/>
+      <c r="K6" s="25"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="64">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
-      <c r="C7" s="62" t="s">
-        <v>113</v>
+      <c r="C7" s="29" t="s">
+        <v>112</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="17">
         <v>0.74</v>
@@ -11129,21 +11489,18 @@
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="65" t="s">
-        <v>114</v>
-      </c>
-      <c r="L7" t="s">
-        <v>118</v>
+      <c r="K7" s="31" t="s">
+        <v>113</v>
       </c>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="64">
+      <c r="B8" s="16">
         <v>2</v>
       </c>
-      <c r="C8" s="63"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="17">
         <v>0.74</v>
@@ -11157,154 +11514,623 @@
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
-      <c r="K8" s="66"/>
+      <c r="K8" s="32"/>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="64">
+      <c r="B9" s="16">
         <v>3</v>
       </c>
-      <c r="C9" s="67" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" s="17">
+      <c r="C9" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="70">
         <v>2.2799999999999998</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="70">
         <f>J9*H9/1000</f>
         <v>154</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="70">
         <v>110</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="70">
         <v>280</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="70">
         <v>200</v>
       </c>
-      <c r="J9" s="68">
-        <f>G9*1000/I9</f>
+      <c r="J9" s="72">
+        <f>ROUND(G9*1000/I9,1)</f>
         <v>550</v>
       </c>
-      <c r="K9" s="68" t="s">
+      <c r="K9" s="70" t="s">
+        <v>120</v>
+      </c>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="16">
+        <v>4</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="71">
+        <v>8.5</v>
+      </c>
+      <c r="F10" s="71">
+        <v>100</v>
+      </c>
+      <c r="G10" s="71">
+        <v>60</v>
+      </c>
+      <c r="H10" s="71">
+        <v>400</v>
+      </c>
+      <c r="I10" s="71">
+        <v>200</v>
+      </c>
+      <c r="J10" s="71">
+        <f>ROUND(G10*1000/I10,1)</f>
+        <v>300</v>
+      </c>
+      <c r="K10" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="16">
+        <v>7</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="64">
-        <v>4</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="73">
+        <v>6.5</v>
+      </c>
+      <c r="F11" s="73">
+        <v>52</v>
+      </c>
+      <c r="G11" s="73">
+        <v>39</v>
+      </c>
+      <c r="H11" s="73">
+        <v>150</v>
+      </c>
+      <c r="I11" s="73">
+        <v>112</v>
+      </c>
+      <c r="J11" s="73">
+        <f>ROUND(G11*1000/I11,1)</f>
+        <v>348.2</v>
+      </c>
+      <c r="K11" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="16">
+        <v>8</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="73">
+        <v>9.5</v>
+      </c>
+      <c r="F12" s="73">
+        <v>105</v>
+      </c>
+      <c r="G12" s="73">
+        <v>79</v>
+      </c>
+      <c r="H12" s="73">
+        <v>300</v>
+      </c>
+      <c r="I12" s="73">
+        <v>225</v>
+      </c>
+      <c r="J12" s="73">
+        <f>ROUND(G12*1000/I12,1)</f>
+        <v>351.1</v>
+      </c>
+      <c r="K12" s="36"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="16">
+        <v>9</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="73">
+        <v>12.5</v>
+      </c>
+      <c r="F13" s="73">
+        <v>157</v>
+      </c>
+      <c r="G13" s="73">
+        <v>118</v>
+      </c>
+      <c r="H13" s="73">
+        <v>450</v>
+      </c>
+      <c r="I13" s="73">
+        <v>337</v>
+      </c>
+      <c r="J13" s="73">
+        <f>ROUND(G13*1000/I13,1)</f>
+        <v>350.1</v>
+      </c>
+      <c r="K13" s="36"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="16">
+        <v>10</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="73">
+        <v>15.5</v>
+      </c>
+      <c r="F14" s="73">
+        <v>212</v>
+      </c>
+      <c r="G14" s="73">
+        <v>160</v>
+      </c>
+      <c r="H14" s="73">
+        <v>600</v>
+      </c>
+      <c r="I14" s="73">
+        <v>450</v>
+      </c>
+      <c r="J14" s="73">
+        <f>ROUND(G14*1000/I14,1)</f>
+        <v>355.6</v>
+      </c>
+      <c r="K14" s="36"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="16">
+        <v>11</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="73">
+        <v>25.2</v>
+      </c>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73">
+        <v>180</v>
+      </c>
+      <c r="H15" s="73">
+        <v>400</v>
+      </c>
+      <c r="I15" s="73">
+        <v>300</v>
+      </c>
+      <c r="J15" s="73">
+        <f>ROUND(G15*1000/I15,1)</f>
+        <v>600</v>
+      </c>
+      <c r="K15" s="36"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="16">
+        <v>12</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="73">
+        <v>29</v>
+      </c>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73">
+        <v>250</v>
+      </c>
+      <c r="H16" s="73">
+        <v>600</v>
+      </c>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="37"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="16">
+        <v>13</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="F17" s="3">
+        <v>16</v>
+      </c>
+      <c r="G17" s="3">
+        <v>12</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="T17" t="s">
+        <v>122</v>
+      </c>
+      <c r="U17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" s="16">
+        <v>14</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="E18" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="F18" s="3">
+        <v>20</v>
+      </c>
+      <c r="G18" s="3">
         <v>16</v>
       </c>
-      <c r="G10" s="4">
-        <v>12</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="L10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="64">
-        <v>5</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="4" t="s">
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="77"/>
+      <c r="K18" s="78"/>
+      <c r="T18">
+        <f xml:space="preserve"> 49.9/398 * (U18-2) + 0.1</f>
+        <v>1.1030150753768846</v>
+      </c>
+      <c r="U18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" s="16">
+        <v>15</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="E19" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="F19" s="3">
+        <v>40</v>
+      </c>
+      <c r="G19" s="3">
+        <v>28</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="78"/>
+      <c r="T19">
+        <f xml:space="preserve"> 49.9/398 * (U19-2) + 0.1</f>
+        <v>2.3567839195979903</v>
+      </c>
+      <c r="U19">
         <v>20</v>
       </c>
-      <c r="G11" s="4">
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" s="16">
         <v>16</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="22"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="64">
-        <v>6</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="4" t="s">
+      <c r="C20" s="28"/>
+      <c r="D20" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="4">
-        <v>3.4</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="E20" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="F20" s="3">
         <v>40</v>
       </c>
-      <c r="G12" s="4">
-        <v>28</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="22"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="64">
-        <v>7</v>
-      </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" s="4">
-        <v>6.8</v>
-      </c>
-      <c r="F13" s="4">
-        <v>40</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="G20" s="3">
         <v>50</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="23"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="80"/>
+      <c r="T20">
+        <f t="shared" ref="T20:T46" si="0" xml:space="preserve"> 49.9/398 * (U20-2) + 0.1</f>
+        <v>3.6105527638190957</v>
+      </c>
+      <c r="U20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T21">
+        <f t="shared" si="0"/>
+        <v>6.1180904522613062</v>
+      </c>
+      <c r="U21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>7.3718592964824126</v>
+      </c>
+      <c r="U22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T23">
+        <f t="shared" si="0"/>
+        <v>8.6256281407035171</v>
+      </c>
+      <c r="U23">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T24">
+        <f t="shared" si="0"/>
+        <v>9.8793969849246235</v>
+      </c>
+      <c r="U24">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T25">
+        <f t="shared" si="0"/>
+        <v>11.13316582914573</v>
+      </c>
+      <c r="U25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>12.386934673366834</v>
+      </c>
+      <c r="U26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T27">
+        <f t="shared" si="0"/>
+        <v>13.640703517587941</v>
+      </c>
+      <c r="U27">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T28">
+        <f t="shared" si="0"/>
+        <v>14.894472361809045</v>
+      </c>
+      <c r="U28">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T29">
+        <f t="shared" si="0"/>
+        <v>16.148241206030153</v>
+      </c>
+      <c r="U29">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T30">
+        <f t="shared" si="0"/>
+        <v>17.40201005025126</v>
+      </c>
+      <c r="U30">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T31">
+        <f t="shared" si="0"/>
+        <v>18.655778894472366</v>
+      </c>
+      <c r="U31">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T32">
+        <f t="shared" si="0"/>
+        <v>19.909547738693469</v>
+      </c>
+      <c r="U32">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T33">
+        <f t="shared" si="0"/>
+        <v>21.163316582914575</v>
+      </c>
+      <c r="U33">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T34">
+        <f t="shared" si="0"/>
+        <v>22.417085427135682</v>
+      </c>
+      <c r="U34">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T35">
+        <f t="shared" si="0"/>
+        <v>23.670854271356788</v>
+      </c>
+      <c r="U35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T36">
+        <f t="shared" si="0"/>
+        <v>24.924623115577894</v>
+      </c>
+      <c r="U36">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T37">
+        <f t="shared" si="0"/>
+        <v>26.178391959798997</v>
+      </c>
+      <c r="U37">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T38">
+        <f t="shared" si="0"/>
+        <v>27.432160804020103</v>
+      </c>
+      <c r="U38">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T39">
+        <f t="shared" si="0"/>
+        <v>28.68592964824121</v>
+      </c>
+      <c r="U39">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T40">
+        <f t="shared" si="0"/>
+        <v>29.939698492462316</v>
+      </c>
+      <c r="U40">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T41">
+        <f t="shared" si="0"/>
+        <v>31.193467336683423</v>
+      </c>
+      <c r="U41">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T42">
+        <f t="shared" si="0"/>
+        <v>32.447236180904525</v>
+      </c>
+      <c r="U42">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T43">
+        <f t="shared" si="0"/>
+        <v>33.701005025125632</v>
+      </c>
+      <c r="U43">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="44" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T44">
+        <f t="shared" si="0"/>
+        <v>34.954773869346738</v>
+      </c>
+      <c r="U44">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T45">
+        <f t="shared" si="0"/>
+        <v>36.208542713567844</v>
+      </c>
+      <c r="U45">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="46" spans="20:21" x14ac:dyDescent="0.2">
+      <c r="T46">
+        <f t="shared" si="0"/>
+        <v>37.462311557788951</v>
+      </c>
+      <c r="U46">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
     <mergeCell ref="B2:K3"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C17:C20"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="K17:K20"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="K11:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -11316,7 +12142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EA9C6B-7942-C84D-BA2E-598934CE2C8D}">
   <dimension ref="B2:Q123"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A81" zoomScale="75" workbookViewId="0">
       <selection activeCell="I109" sqref="I109:K111"/>
     </sheetView>
   </sheetViews>
@@ -11333,19 +12159,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
@@ -11353,17 +12179,17 @@
       <c r="Q2" s="15"/>
     </row>
     <row r="3" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
       <c r="M3" s="15"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
@@ -11380,62 +12206,62 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="24" t="s">
+      <c r="J5" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="24" t="s">
-        <v>20</v>
+      <c r="L5" s="25" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="16">
         <v>1</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>76</v>
       </c>
       <c r="E7" s="17">
         <v>14.5</v>
@@ -11462,17 +12288,17 @@
         <f>ROUND(9550*G7/I7,1)</f>
         <v>5968.8</v>
       </c>
-      <c r="L7" s="34" t="s">
-        <v>79</v>
+      <c r="L7" s="64" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="16">
         <v>2</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="17">
         <v>27</v>
@@ -11499,15 +12325,15 @@
         <f>ROUND(9550*G8/I8,1)</f>
         <v>4004.8</v>
       </c>
-      <c r="L8" s="35"/>
+      <c r="L8" s="65"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="16">
         <v>3</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="17">
         <v>48</v>
@@ -11534,13 +12360,13 @@
         <f>ROUND(9550*G9/I9,1)</f>
         <v>3660.8</v>
       </c>
-      <c r="L9" s="36"/>
+      <c r="L9" s="66"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="16">
         <v>4</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="43" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="9">
@@ -11571,15 +12397,15 @@
         <f>ROUND(9550*G10/I10,1)</f>
         <v>6309.8</v>
       </c>
-      <c r="L10" s="30" t="s">
-        <v>63</v>
+      <c r="L10" s="46" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="16">
         <v>5</v>
       </c>
-      <c r="C11" s="42"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="9">
         <v>208</v>
       </c>
@@ -11608,13 +12434,13 @@
         <f t="shared" ref="K11:K41" si="3">ROUND(9550*G11/I11,1)</f>
         <v>5942.2</v>
       </c>
-      <c r="L11" s="30"/>
+      <c r="L11" s="46"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="16">
         <v>6</v>
       </c>
-      <c r="C12" s="42"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="9">
         <v>228</v>
       </c>
@@ -11643,13 +12469,13 @@
         <f t="shared" si="3"/>
         <v>5509.6</v>
       </c>
-      <c r="L12" s="30"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="16">
         <v>7</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="9">
         <v>268</v>
       </c>
@@ -11678,13 +12504,13 @@
         <f t="shared" si="3"/>
         <v>4469.3999999999996</v>
       </c>
-      <c r="L13" s="30"/>
+      <c r="L13" s="46"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="16">
         <v>8</v>
       </c>
-      <c r="C14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="9">
         <v>348</v>
       </c>
@@ -11713,17 +12539,17 @@
         <f t="shared" si="3"/>
         <v>4011</v>
       </c>
-      <c r="L14" s="30"/>
+      <c r="L14" s="46"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="16">
         <v>9</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="E15" s="7">
         <v>3.8</v>
@@ -11750,17 +12576,17 @@
       <c r="K15" s="7">
         <v>2100</v>
       </c>
-      <c r="L15" s="45" t="s">
-        <v>108</v>
+      <c r="L15" s="67" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B16" s="16">
         <v>10</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" s="7">
         <v>4</v>
@@ -11787,15 +12613,15 @@
       <c r="K16" s="7">
         <v>2800</v>
       </c>
-      <c r="L16" s="46"/>
+      <c r="L16" s="68"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="16">
         <v>11</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E17" s="7">
         <v>5.5</v>
@@ -11822,15 +12648,15 @@
       <c r="K17" s="7">
         <v>2200</v>
       </c>
-      <c r="L17" s="46"/>
+      <c r="L17" s="68"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="16">
         <v>12</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" s="7">
         <v>5.5</v>
@@ -11857,15 +12683,15 @@
       <c r="K18" s="7">
         <v>2230</v>
       </c>
-      <c r="L18" s="46"/>
+      <c r="L18" s="68"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="16">
         <v>13</v>
       </c>
-      <c r="C19" s="28"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E19" s="7">
         <v>5.8</v>
@@ -11892,15 +12718,15 @@
       <c r="K19" s="7">
         <v>2700</v>
       </c>
-      <c r="L19" s="46"/>
+      <c r="L19" s="68"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="16">
         <v>14</v>
       </c>
-      <c r="C20" s="28"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20" s="7">
         <v>6</v>
@@ -11927,15 +12753,15 @@
       <c r="K20" s="7">
         <v>2700</v>
       </c>
-      <c r="L20" s="46"/>
+      <c r="L20" s="68"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="16">
         <v>15</v>
       </c>
-      <c r="C21" s="28"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E21" s="7">
         <v>7</v>
@@ -11962,15 +12788,15 @@
       <c r="K21" s="7">
         <v>2250</v>
       </c>
-      <c r="L21" s="46"/>
+      <c r="L21" s="68"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="16">
         <v>16</v>
       </c>
-      <c r="C22" s="28"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E22" s="7">
         <v>11.8</v>
@@ -11997,15 +12823,15 @@
       <c r="K22" s="7">
         <v>2200</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="68"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="16">
         <v>17</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E23" s="7">
         <v>12.8</v>
@@ -12032,15 +12858,15 @@
       <c r="K23" s="7">
         <v>2700</v>
       </c>
-      <c r="L23" s="46"/>
+      <c r="L23" s="68"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="16">
         <v>18</v>
       </c>
-      <c r="C24" s="29"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E24" s="7">
         <v>15.8</v>
@@ -12067,17 +12893,17 @@
       <c r="K24" s="7">
         <v>2700</v>
       </c>
-      <c r="L24" s="47"/>
+      <c r="L24" s="69"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="16">
         <v>19</v>
       </c>
-      <c r="C25" s="27" t="s">
-        <v>93</v>
+      <c r="C25" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E25" s="4">
         <v>4.0999999999999996</v>
@@ -12095,17 +12921,17 @@
         <f t="shared" si="3"/>
         <v>19946.2</v>
       </c>
-      <c r="L25" s="21" t="s">
-        <v>94</v>
+      <c r="L25" s="35" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="16">
         <v>20</v>
       </c>
-      <c r="C26" s="29"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" s="4">
         <v>18.7</v>
@@ -12123,17 +12949,17 @@
         <f t="shared" si="3"/>
         <v>2975.1</v>
       </c>
-      <c r="L26" s="23"/>
+      <c r="L26" s="37"/>
     </row>
     <row r="27" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="16">
         <v>21</v>
       </c>
-      <c r="C27" s="39" t="s">
-        <v>15</v>
+      <c r="C27" s="61" t="s">
+        <v>14</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" s="19">
         <v>1.8</v>
@@ -12160,17 +12986,17 @@
         <f>ROUND(9550*G27/I27,1)</f>
         <v>6023.8</v>
       </c>
-      <c r="L27" s="40" t="s">
-        <v>21</v>
+      <c r="L27" s="44" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="16">
         <v>22</v>
       </c>
-      <c r="C28" s="39"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28" s="19">
         <v>2.75</v>
@@ -12197,15 +13023,15 @@
         <f t="shared" ref="K28:K31" si="5">ROUND(9550*G28/I28,1)</f>
         <v>6002.9</v>
       </c>
-      <c r="L28" s="40"/>
+      <c r="L28" s="44"/>
     </row>
     <row r="29" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="16">
         <v>23</v>
       </c>
-      <c r="C29" s="39"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="19">
         <v>3.35</v>
@@ -12232,15 +13058,15 @@
         <f t="shared" si="5"/>
         <v>2506.9</v>
       </c>
-      <c r="L29" s="40"/>
+      <c r="L29" s="44"/>
     </row>
     <row r="30" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" s="16">
         <v>24</v>
       </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E30" s="19">
         <v>4</v>
@@ -12267,15 +13093,15 @@
         <f t="shared" si="5"/>
         <v>2522.6</v>
       </c>
-      <c r="L30" s="40"/>
+      <c r="L30" s="44"/>
     </row>
     <row r="31" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="16">
         <v>25</v>
       </c>
-      <c r="C31" s="39"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" s="19">
         <v>22</v>
@@ -12302,17 +13128,17 @@
         <f t="shared" si="5"/>
         <v>2247.1</v>
       </c>
-      <c r="L31" s="40"/>
+      <c r="L31" s="44"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="16">
         <v>26</v>
       </c>
-      <c r="C32" s="39" t="s">
-        <v>19</v>
+      <c r="C32" s="61" t="s">
+        <v>18</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" s="20">
         <v>1.56</v>
@@ -12339,17 +13165,17 @@
       <c r="K32" s="5">
         <v>6250</v>
       </c>
-      <c r="L32" s="41" t="s">
-        <v>22</v>
+      <c r="L32" s="45" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B33" s="16">
         <v>27</v>
       </c>
-      <c r="C33" s="39"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E33" s="20">
         <v>5.78</v>
@@ -12376,17 +13202,17 @@
       <c r="K33" s="5">
         <v>6500</v>
       </c>
-      <c r="L33" s="41"/>
+      <c r="L33" s="45"/>
     </row>
     <row r="34" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="16">
         <v>28</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="E34" s="9">
         <v>1.1000000000000001</v>
@@ -12413,17 +13239,17 @@
         <f t="shared" si="3"/>
         <v>4340.8999999999996</v>
       </c>
-      <c r="L34" s="30" t="s">
-        <v>32</v>
+      <c r="L34" s="46" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="16">
         <v>29</v>
       </c>
-      <c r="C35" s="42"/>
+      <c r="C35" s="43"/>
       <c r="D35" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E35" s="9">
         <v>2.25</v>
@@ -12450,15 +13276,15 @@
         <f t="shared" si="3"/>
         <v>3350.9</v>
       </c>
-      <c r="L35" s="30"/>
+      <c r="L35" s="46"/>
     </row>
     <row r="36" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="16">
         <v>30</v>
       </c>
-      <c r="C36" s="42"/>
+      <c r="C36" s="43"/>
       <c r="D36" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E36" s="9">
         <v>4.5</v>
@@ -12485,15 +13311,15 @@
         <f t="shared" si="3"/>
         <v>2546.6999999999998</v>
       </c>
-      <c r="L36" s="30"/>
+      <c r="L36" s="46"/>
     </row>
     <row r="37" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" s="16">
         <v>31</v>
       </c>
-      <c r="C37" s="42"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E37" s="9">
         <v>7.5</v>
@@ -12520,15 +13346,15 @@
         <f t="shared" si="3"/>
         <v>2494.6999999999998</v>
       </c>
-      <c r="L37" s="30"/>
+      <c r="L37" s="46"/>
     </row>
     <row r="38" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B38" s="16">
         <v>32</v>
       </c>
-      <c r="C38" s="42"/>
+      <c r="C38" s="43"/>
       <c r="D38" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E38" s="9">
         <v>14.25</v>
@@ -12555,15 +13381,15 @@
         <f t="shared" si="3"/>
         <v>1942.4</v>
       </c>
-      <c r="L38" s="30"/>
+      <c r="L38" s="46"/>
     </row>
     <row r="39" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="16">
         <v>33</v>
       </c>
-      <c r="C39" s="42"/>
+      <c r="C39" s="43"/>
       <c r="D39" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E39" s="9">
         <v>25.5</v>
@@ -12590,15 +13416,15 @@
         <f t="shared" si="3"/>
         <v>1637.1</v>
       </c>
-      <c r="L39" s="30"/>
+      <c r="L39" s="46"/>
     </row>
     <row r="40" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" s="16">
         <v>34</v>
       </c>
-      <c r="C40" s="42"/>
+      <c r="C40" s="43"/>
       <c r="D40" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E40" s="9">
         <v>45</v>
@@ -12625,15 +13451,15 @@
         <f t="shared" si="3"/>
         <v>1597.2</v>
       </c>
-      <c r="L40" s="30"/>
+      <c r="L40" s="46"/>
     </row>
     <row r="41" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="16">
         <v>35</v>
       </c>
-      <c r="C41" s="42"/>
+      <c r="C41" s="43"/>
       <c r="D41" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E41" s="9">
         <v>75</v>
@@ -12660,17 +13486,17 @@
         <f t="shared" si="3"/>
         <v>1284</v>
       </c>
-      <c r="L41" s="30"/>
+      <c r="L41" s="46"/>
     </row>
     <row r="42" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B42" s="16">
         <v>36</v>
       </c>
-      <c r="C42" s="39" t="s">
-        <v>41</v>
+      <c r="C42" s="61" t="s">
+        <v>40</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E42" s="11">
         <v>53</v>
@@ -12697,15 +13523,15 @@
       <c r="K42" s="11">
         <v>2500</v>
       </c>
-      <c r="L42" s="38" t="s">
-        <v>42</v>
+      <c r="L42" s="53" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" s="16">
         <v>37</v>
       </c>
-      <c r="C43" s="39"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="11">
         <v>250</v>
       </c>
@@ -12734,13 +13560,13 @@
         <f>ROUND(9550*G43/I43,1)</f>
         <v>1900.5</v>
       </c>
-      <c r="L43" s="38"/>
+      <c r="L43" s="53"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B44" s="16">
         <v>38</v>
       </c>
-      <c r="C44" s="39"/>
+      <c r="C44" s="61"/>
       <c r="D44" s="11">
         <v>500</v>
       </c>
@@ -12769,17 +13595,17 @@
         <f>ROUND(9550*G44/I44,1)</f>
         <v>1900.5</v>
       </c>
-      <c r="L44" s="38"/>
+      <c r="L44" s="53"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" s="16">
         <v>39</v>
       </c>
-      <c r="C45" s="27" t="s">
-        <v>92</v>
+      <c r="C45" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E45" s="4">
         <v>3.1</v>
@@ -12806,17 +13632,17 @@
         <f>ROUND(9550*G45/I45,1)</f>
         <v>3820</v>
       </c>
-      <c r="L45" s="21" t="s">
-        <v>91</v>
+      <c r="L45" s="35" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B46" s="16">
         <v>40</v>
       </c>
-      <c r="C46" s="28"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E46" s="4">
         <v>3.75</v>
@@ -12843,15 +13669,15 @@
         <f t="shared" ref="K46:K55" si="7">ROUND(9550*G46/I46,1)</f>
         <v>3274.3</v>
       </c>
-      <c r="L46" s="22"/>
+      <c r="L46" s="36"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B47" s="16">
         <v>41</v>
       </c>
-      <c r="C47" s="28"/>
+      <c r="C47" s="27"/>
       <c r="D47" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E47" s="4">
         <v>4</v>
@@ -12878,15 +13704,15 @@
         <f t="shared" si="7"/>
         <v>3274.3</v>
       </c>
-      <c r="L47" s="22"/>
+      <c r="L47" s="36"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B48" s="16">
         <v>42</v>
       </c>
-      <c r="C48" s="28"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E48" s="4">
         <v>5.25</v>
@@ -12913,15 +13739,15 @@
         <f t="shared" si="7"/>
         <v>2319.3000000000002</v>
       </c>
-      <c r="L48" s="22"/>
+      <c r="L48" s="36"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B49" s="16">
         <v>43</v>
       </c>
-      <c r="C49" s="28"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E49" s="4">
         <v>7.5</v>
@@ -12948,15 +13774,15 @@
         <f t="shared" si="7"/>
         <v>2387.5</v>
       </c>
-      <c r="L49" s="22"/>
+      <c r="L49" s="36"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B50" s="16">
         <v>44</v>
       </c>
-      <c r="C50" s="28"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E50" s="4">
         <v>8</v>
@@ -12983,15 +13809,15 @@
         <f t="shared" si="7"/>
         <v>1989.6</v>
       </c>
-      <c r="L50" s="22"/>
+      <c r="L50" s="36"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B51" s="16">
         <v>45</v>
       </c>
-      <c r="C51" s="28"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E51" s="4">
         <v>8.15</v>
@@ -13018,15 +13844,15 @@
         <f t="shared" si="7"/>
         <v>1910</v>
       </c>
-      <c r="L51" s="22"/>
+      <c r="L51" s="36"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B52" s="16">
         <v>46</v>
       </c>
-      <c r="C52" s="28"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E52" s="4">
         <v>12</v>
@@ -13053,15 +13879,15 @@
         <f t="shared" si="7"/>
         <v>1910</v>
       </c>
-      <c r="L52" s="22"/>
+      <c r="L52" s="36"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B53" s="16">
         <v>47</v>
       </c>
-      <c r="C53" s="28"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E53" s="4">
         <v>15.3</v>
@@ -13088,15 +13914,15 @@
         <f t="shared" si="7"/>
         <v>1719</v>
       </c>
-      <c r="L53" s="22"/>
+      <c r="L53" s="36"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B54" s="16">
         <v>48</v>
       </c>
-      <c r="C54" s="28"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E54" s="4">
         <v>17.3</v>
@@ -13123,15 +13949,15 @@
         <f t="shared" si="7"/>
         <v>2387.5</v>
       </c>
-      <c r="L54" s="22"/>
+      <c r="L54" s="36"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B55" s="16">
         <v>49</v>
       </c>
-      <c r="C55" s="29"/>
+      <c r="C55" s="28"/>
       <c r="D55" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E55" s="4">
         <v>23.8</v>
@@ -13158,14 +13984,14 @@
         <f t="shared" si="7"/>
         <v>2228.3000000000002</v>
       </c>
-      <c r="L55" s="23"/>
+      <c r="L55" s="37"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B56" s="16">
         <v>50</v>
       </c>
-      <c r="C56" s="42" t="s">
-        <v>43</v>
+      <c r="C56" s="43" t="s">
+        <v>42</v>
       </c>
       <c r="D56" s="3">
         <v>8019</v>
@@ -13195,15 +14021,15 @@
         <f t="shared" ref="K56:K60" si="8">ROUND(9550*G56/I56,1)</f>
         <v>#N/A</v>
       </c>
-      <c r="L56" s="40" t="s">
-        <v>44</v>
+      <c r="L56" s="44" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B57" s="16">
         <v>51</v>
       </c>
-      <c r="C57" s="42"/>
+      <c r="C57" s="43"/>
       <c r="D57" s="3">
         <v>8025</v>
       </c>
@@ -13232,13 +14058,13 @@
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-      <c r="L57" s="40"/>
+      <c r="L57" s="44"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B58" s="16">
         <v>52</v>
       </c>
-      <c r="C58" s="42"/>
+      <c r="C58" s="43"/>
       <c r="D58" s="3">
         <v>8038</v>
       </c>
@@ -13267,13 +14093,13 @@
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-      <c r="L58" s="40"/>
+      <c r="L58" s="44"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B59" s="16">
         <v>53</v>
       </c>
-      <c r="C59" s="42"/>
+      <c r="C59" s="43"/>
       <c r="D59" s="3">
         <v>8057</v>
       </c>
@@ -13302,13 +14128,13 @@
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-      <c r="L59" s="40"/>
+      <c r="L59" s="44"/>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B60" s="16">
         <v>54</v>
       </c>
-      <c r="C60" s="42"/>
+      <c r="C60" s="43"/>
       <c r="D60" s="3">
         <v>12030</v>
       </c>
@@ -13337,17 +14163,17 @@
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-      <c r="L60" s="40"/>
+      <c r="L60" s="44"/>
     </row>
     <row r="61" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B61" s="16">
         <v>55</v>
       </c>
-      <c r="C61" s="42" t="s">
-        <v>48</v>
+      <c r="C61" s="43" t="s">
+        <v>47</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E61" s="5">
         <v>8.5</v>
@@ -13374,17 +14200,17 @@
       <c r="K61" s="5">
         <v>3000</v>
       </c>
-      <c r="L61" s="41" t="s">
-        <v>65</v>
+      <c r="L61" s="45" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="16">
         <v>56</v>
       </c>
-      <c r="C62" s="42"/>
+      <c r="C62" s="43"/>
       <c r="D62" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E62" s="5">
         <v>1.45</v>
@@ -13411,15 +14237,15 @@
       <c r="K62" s="5">
         <v>6000</v>
       </c>
-      <c r="L62" s="41"/>
+      <c r="L62" s="45"/>
     </row>
     <row r="63" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B63" s="16">
         <v>57</v>
       </c>
-      <c r="C63" s="42"/>
+      <c r="C63" s="43"/>
       <c r="D63" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E63" s="5">
         <v>1.95</v>
@@ -13446,17 +14272,17 @@
       <c r="K63" s="5">
         <v>6000</v>
       </c>
-      <c r="L63" s="41"/>
+      <c r="L63" s="45"/>
     </row>
     <row r="64" spans="2:12" ht="34" x14ac:dyDescent="0.2">
       <c r="B64" s="16">
         <v>58</v>
       </c>
       <c r="C64" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="E64" s="9">
         <v>18</v>
@@ -13484,18 +14310,18 @@
         <v>2500</v>
       </c>
       <c r="L64" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B65" s="16">
         <v>59</v>
       </c>
-      <c r="C65" s="42" t="s">
-        <v>51</v>
+      <c r="C65" s="43" t="s">
+        <v>50</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E65" s="11">
         <v>13</v>
@@ -13522,17 +14348,17 @@
       <c r="K65" s="11">
         <v>2500</v>
       </c>
-      <c r="L65" s="38" t="s">
-        <v>52</v>
+      <c r="L65" s="53" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" s="16">
         <v>60</v>
       </c>
-      <c r="C66" s="42"/>
+      <c r="C66" s="43"/>
       <c r="D66" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E66" s="11">
         <v>50</v>
@@ -13558,17 +14384,17 @@
       <c r="K66" s="11">
         <v>2500</v>
       </c>
-      <c r="L66" s="38"/>
+      <c r="L66" s="53"/>
     </row>
     <row r="67" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B67" s="16">
         <v>61</v>
       </c>
-      <c r="C67" s="27" t="s">
+      <c r="C67" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="E67" s="12">
         <v>3.6</v>
@@ -13587,17 +14413,17 @@
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
       <c r="K67" s="12"/>
-      <c r="L67" s="21" t="s">
-        <v>73</v>
+      <c r="L67" s="35" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B68" s="16">
         <v>62</v>
       </c>
-      <c r="C68" s="28"/>
+      <c r="C68" s="27"/>
       <c r="D68" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E68" s="12">
         <v>4.4080000000000004</v>
@@ -13616,15 +14442,15 @@
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
       <c r="K68" s="12"/>
-      <c r="L68" s="22"/>
+      <c r="L68" s="36"/>
     </row>
     <row r="69" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B69" s="16">
         <v>63</v>
       </c>
-      <c r="C69" s="29"/>
+      <c r="C69" s="28"/>
       <c r="D69" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E69" s="12">
         <v>5.13</v>
@@ -13643,17 +14469,17 @@
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
       <c r="K69" s="12"/>
-      <c r="L69" s="23"/>
+      <c r="L69" s="37"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B70" s="16">
         <v>64</v>
       </c>
-      <c r="C70" s="42" t="s">
+      <c r="C70" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="E70" s="3">
         <v>1.179</v>
@@ -13680,17 +14506,17 @@
         <f t="shared" ref="K70:K72" si="10">ROUND(9550*G70/I70,1)</f>
         <v>8011.7</v>
       </c>
-      <c r="L70" s="40" t="s">
-        <v>60</v>
+      <c r="L70" s="44" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B71" s="16">
         <v>65</v>
       </c>
-      <c r="C71" s="42"/>
+      <c r="C71" s="43"/>
       <c r="D71" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E71" s="3">
         <v>1.27</v>
@@ -13717,15 +14543,15 @@
         <f t="shared" si="10"/>
         <v>8003.2</v>
       </c>
-      <c r="L71" s="40"/>
+      <c r="L71" s="44"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B72" s="16">
         <v>66</v>
       </c>
-      <c r="C72" s="42"/>
+      <c r="C72" s="43"/>
       <c r="D72" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E72" s="3">
         <v>1.5880000000000001</v>
@@ -13752,17 +14578,17 @@
         <f t="shared" si="10"/>
         <v>7988</v>
       </c>
-      <c r="L72" s="40"/>
+      <c r="L72" s="44"/>
     </row>
     <row r="73" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B73" s="16">
         <v>67</v>
       </c>
-      <c r="C73" s="42" t="s">
+      <c r="C73" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="E73" s="8">
         <v>4.5</v>
@@ -13789,17 +14615,17 @@
       <c r="K73" s="8">
         <v>2400</v>
       </c>
-      <c r="L73" s="41" t="s">
-        <v>39</v>
+      <c r="L73" s="45" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B74" s="16">
         <v>68</v>
       </c>
-      <c r="C74" s="42"/>
+      <c r="C74" s="43"/>
       <c r="D74" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E74" s="8">
         <v>6</v>
@@ -13826,15 +14652,15 @@
       <c r="K74" s="8">
         <v>2000</v>
       </c>
-      <c r="L74" s="41"/>
+      <c r="L74" s="45"/>
     </row>
     <row r="75" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B75" s="16">
         <v>69</v>
       </c>
-      <c r="C75" s="42"/>
+      <c r="C75" s="43"/>
       <c r="D75" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E75" s="8">
         <v>8.1999999999999993</v>
@@ -13861,15 +14687,15 @@
       <c r="K75" s="8">
         <v>2400</v>
       </c>
-      <c r="L75" s="41"/>
+      <c r="L75" s="45"/>
     </row>
     <row r="76" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B76" s="16">
         <v>70</v>
       </c>
-      <c r="C76" s="42"/>
+      <c r="C76" s="43"/>
       <c r="D76" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E76" s="8">
         <v>9.8000000000000007</v>
@@ -13896,15 +14722,15 @@
       <c r="K76" s="8">
         <v>2000</v>
       </c>
-      <c r="L76" s="41"/>
+      <c r="L76" s="45"/>
     </row>
     <row r="77" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B77" s="16">
         <v>71</v>
       </c>
-      <c r="C77" s="42"/>
+      <c r="C77" s="43"/>
       <c r="D77" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E77" s="8">
         <v>19</v>
@@ -13931,15 +14757,15 @@
       <c r="K77" s="8">
         <v>2400</v>
       </c>
-      <c r="L77" s="41"/>
+      <c r="L77" s="45"/>
     </row>
     <row r="78" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B78" s="16">
         <v>72</v>
       </c>
-      <c r="C78" s="42"/>
+      <c r="C78" s="43"/>
       <c r="D78" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E78" s="8">
         <v>30</v>
@@ -13966,7 +14792,7 @@
       <c r="K78" s="8">
         <v>2400</v>
       </c>
-      <c r="L78" s="41"/>
+      <c r="L78" s="45"/>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B79" s="14"/>
@@ -14021,82 +14847,82 @@
       <c r="L82" s="14"/>
     </row>
     <row r="83" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="C83" s="61"/>
-      <c r="D83" s="61"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="61"/>
-      <c r="G83" s="61"/>
-      <c r="H83" s="61"/>
-      <c r="I83" s="61"/>
-      <c r="J83" s="61"/>
-      <c r="K83" s="61"/>
+      <c r="B83" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="42"/>
+      <c r="F83" s="42"/>
+      <c r="G83" s="42"/>
+      <c r="H83" s="42"/>
+      <c r="I83" s="42"/>
+      <c r="J83" s="42"/>
+      <c r="K83" s="42"/>
       <c r="L83" s="18"/>
     </row>
     <row r="84" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="61"/>
-      <c r="C84" s="61"/>
-      <c r="D84" s="61"/>
-      <c r="E84" s="61"/>
-      <c r="F84" s="61"/>
-      <c r="G84" s="61"/>
-      <c r="H84" s="61"/>
-      <c r="I84" s="61"/>
-      <c r="J84" s="61"/>
-      <c r="K84" s="61"/>
+      <c r="B84" s="42"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="42"/>
+      <c r="I84" s="42"/>
+      <c r="J84" s="42"/>
+      <c r="K84" s="42"/>
       <c r="L84" s="18"/>
     </row>
     <row r="86" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="24" t="s">
+      <c r="B86" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C86" s="24" t="s">
+      <c r="C86" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D86" s="24" t="s">
+      <c r="D86" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E86" s="24" t="s">
+      <c r="E86" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F86" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G86" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F86" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="G86" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H86" s="24" t="s">
+      <c r="H86" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I86" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="J86" s="60"/>
-      <c r="K86" s="60"/>
+      <c r="I86" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J86" s="41"/>
+      <c r="K86" s="41"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
-      <c r="H87" s="24"/>
-      <c r="I87" s="60"/>
-      <c r="J87" s="60"/>
-      <c r="K87" s="60"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="25"/>
+      <c r="I87" s="41"/>
+      <c r="J87" s="41"/>
+      <c r="K87" s="41"/>
     </row>
     <row r="88" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="16">
         <v>1</v>
       </c>
-      <c r="C88" s="31" t="s">
+      <c r="C88" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D88" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="D88" s="17" t="s">
-        <v>76</v>
       </c>
       <c r="E88" s="17">
         <v>14.5</v>
@@ -14111,19 +14937,19 @@
         <f t="shared" ref="H88:H101" si="12">ROUND(9550*F88/G88,1)</f>
         <v>5968.8</v>
       </c>
-      <c r="I88" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="J88" s="44"/>
-      <c r="K88" s="44"/>
+      <c r="I88" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="J88" s="54"/>
+      <c r="K88" s="54"/>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B89" s="16">
         <v>2</v>
       </c>
-      <c r="C89" s="32"/>
+      <c r="C89" s="39"/>
       <c r="D89" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E89" s="17">
         <v>27</v>
@@ -14138,17 +14964,17 @@
         <f t="shared" si="12"/>
         <v>4004.8</v>
       </c>
-      <c r="I89" s="44"/>
-      <c r="J89" s="44"/>
-      <c r="K89" s="44"/>
+      <c r="I89" s="54"/>
+      <c r="J89" s="54"/>
+      <c r="K89" s="54"/>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B90" s="16">
         <v>3</v>
       </c>
-      <c r="C90" s="33"/>
+      <c r="C90" s="40"/>
       <c r="D90" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E90" s="17">
         <v>48</v>
@@ -14163,15 +14989,15 @@
         <f t="shared" si="12"/>
         <v>3660.8</v>
       </c>
-      <c r="I90" s="44"/>
-      <c r="J90" s="44"/>
-      <c r="K90" s="44"/>
+      <c r="I90" s="54"/>
+      <c r="J90" s="54"/>
+      <c r="K90" s="54"/>
     </row>
     <row r="91" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="16">
         <v>4</v>
       </c>
-      <c r="C91" s="42" t="s">
+      <c r="C91" s="43" t="s">
         <v>8</v>
       </c>
       <c r="D91" s="9">
@@ -14190,17 +15016,17 @@
         <f t="shared" si="12"/>
         <v>6309.8</v>
       </c>
-      <c r="I91" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="J91" s="30"/>
-      <c r="K91" s="30"/>
+      <c r="I91" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="J91" s="46"/>
+      <c r="K91" s="46"/>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B92" s="16">
         <v>5</v>
       </c>
-      <c r="C92" s="42"/>
+      <c r="C92" s="43"/>
       <c r="D92" s="9">
         <v>208</v>
       </c>
@@ -14217,15 +15043,15 @@
         <f t="shared" si="12"/>
         <v>5942.2</v>
       </c>
-      <c r="I92" s="30"/>
-      <c r="J92" s="30"/>
-      <c r="K92" s="30"/>
+      <c r="I92" s="46"/>
+      <c r="J92" s="46"/>
+      <c r="K92" s="46"/>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B93" s="16">
         <v>6</v>
       </c>
-      <c r="C93" s="42"/>
+      <c r="C93" s="43"/>
       <c r="D93" s="9">
         <v>228</v>
       </c>
@@ -14242,15 +15068,15 @@
         <f t="shared" si="12"/>
         <v>5509.6</v>
       </c>
-      <c r="I93" s="30"/>
-      <c r="J93" s="30"/>
-      <c r="K93" s="30"/>
+      <c r="I93" s="46"/>
+      <c r="J93" s="46"/>
+      <c r="K93" s="46"/>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B94" s="16">
         <v>7</v>
       </c>
-      <c r="C94" s="42"/>
+      <c r="C94" s="43"/>
       <c r="D94" s="9">
         <v>268</v>
       </c>
@@ -14267,15 +15093,15 @@
         <f t="shared" si="12"/>
         <v>4469.3999999999996</v>
       </c>
-      <c r="I94" s="30"/>
-      <c r="J94" s="30"/>
-      <c r="K94" s="30"/>
+      <c r="I94" s="46"/>
+      <c r="J94" s="46"/>
+      <c r="K94" s="46"/>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B95" s="16">
         <v>8</v>
       </c>
-      <c r="C95" s="42"/>
+      <c r="C95" s="43"/>
       <c r="D95" s="9">
         <v>348</v>
       </c>
@@ -14292,19 +15118,19 @@
         <f t="shared" si="12"/>
         <v>4011</v>
       </c>
-      <c r="I95" s="30"/>
-      <c r="J95" s="30"/>
-      <c r="K95" s="30"/>
+      <c r="I95" s="46"/>
+      <c r="J95" s="46"/>
+      <c r="K95" s="46"/>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B96" s="16">
         <v>9</v>
       </c>
-      <c r="C96" s="28" t="s">
-        <v>97</v>
+      <c r="C96" s="27" t="s">
+        <v>96</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E96" s="7">
         <v>5.8</v>
@@ -14319,19 +15145,19 @@
       <c r="H96" s="7">
         <v>2700</v>
       </c>
-      <c r="I96" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="J96" s="49"/>
-      <c r="K96" s="50"/>
+      <c r="I96" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="J96" s="56"/>
+      <c r="K96" s="57"/>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" s="16">
         <v>10</v>
       </c>
-      <c r="C97" s="28"/>
+      <c r="C97" s="27"/>
       <c r="D97" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E97" s="7">
         <v>12.8</v>
@@ -14346,17 +15172,17 @@
       <c r="H97" s="7">
         <v>2700</v>
       </c>
-      <c r="I97" s="48"/>
-      <c r="J97" s="49"/>
-      <c r="K97" s="50"/>
+      <c r="I97" s="55"/>
+      <c r="J97" s="56"/>
+      <c r="K97" s="57"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B98" s="16">
         <v>11</v>
       </c>
-      <c r="C98" s="29"/>
+      <c r="C98" s="28"/>
       <c r="D98" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E98" s="7">
         <v>15.8</v>
@@ -14371,19 +15197,19 @@
       <c r="H98" s="7">
         <v>2700</v>
       </c>
-      <c r="I98" s="51"/>
-      <c r="J98" s="52"/>
-      <c r="K98" s="53"/>
+      <c r="I98" s="58"/>
+      <c r="J98" s="59"/>
+      <c r="K98" s="60"/>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B99" s="16">
         <v>12</v>
       </c>
-      <c r="C99" s="27" t="s">
-        <v>93</v>
+      <c r="C99" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E99" s="4">
         <v>4.0999999999999996</v>
@@ -14398,19 +15224,19 @@
         <f t="shared" si="12"/>
         <v>19946.2</v>
       </c>
-      <c r="I99" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="J99" s="55"/>
-      <c r="K99" s="56"/>
+      <c r="I99" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="J99" s="48"/>
+      <c r="K99" s="49"/>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B100" s="16">
         <v>13</v>
       </c>
-      <c r="C100" s="29"/>
+      <c r="C100" s="28"/>
       <c r="D100" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E100" s="4">
         <v>18.7</v>
@@ -14425,19 +15251,19 @@
         <f t="shared" si="12"/>
         <v>2975.1</v>
       </c>
-      <c r="I100" s="57"/>
-      <c r="J100" s="58"/>
-      <c r="K100" s="59"/>
+      <c r="I100" s="50"/>
+      <c r="J100" s="51"/>
+      <c r="K100" s="52"/>
     </row>
     <row r="101" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="16">
         <v>14</v>
       </c>
       <c r="C101" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="D101" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="E101" s="19">
         <v>22</v>
@@ -14452,21 +15278,21 @@
         <f t="shared" si="12"/>
         <v>2247.1</v>
       </c>
-      <c r="I101" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J101" s="40"/>
-      <c r="K101" s="40"/>
+      <c r="I101" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J101" s="44"/>
+      <c r="K101" s="44"/>
     </row>
     <row r="102" spans="2:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="16">
         <v>15</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E102" s="20">
         <v>5.78</v>
@@ -14481,21 +15307,21 @@
       <c r="H102" s="5">
         <v>6500</v>
       </c>
-      <c r="I102" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="J102" s="41"/>
-      <c r="K102" s="41"/>
+      <c r="I102" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="J102" s="45"/>
+      <c r="K102" s="45"/>
     </row>
     <row r="103" spans="2:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="16">
         <v>16</v>
       </c>
-      <c r="C103" s="42" t="s">
-        <v>23</v>
+      <c r="C103" s="43" t="s">
+        <v>22</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E103" s="9">
         <v>4.5</v>
@@ -14510,19 +15336,19 @@
         <f t="shared" ref="H103:H108" si="14">ROUND(9550*F103/G103,1)</f>
         <v>2546.6999999999998</v>
       </c>
-      <c r="I103" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="J103" s="30"/>
-      <c r="K103" s="30"/>
+      <c r="I103" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="J103" s="46"/>
+      <c r="K103" s="46"/>
     </row>
     <row r="104" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B104" s="16">
         <v>17</v>
       </c>
-      <c r="C104" s="42"/>
+      <c r="C104" s="43"/>
       <c r="D104" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E104" s="9">
         <v>7.5</v>
@@ -14537,17 +15363,17 @@
         <f t="shared" si="14"/>
         <v>2494.6999999999998</v>
       </c>
-      <c r="I104" s="30"/>
-      <c r="J104" s="30"/>
-      <c r="K104" s="30"/>
+      <c r="I104" s="46"/>
+      <c r="J104" s="46"/>
+      <c r="K104" s="46"/>
     </row>
     <row r="105" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B105" s="16">
         <v>18</v>
       </c>
-      <c r="C105" s="42"/>
+      <c r="C105" s="43"/>
       <c r="D105" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E105" s="9">
         <v>14.25</v>
@@ -14562,17 +15388,17 @@
         <f t="shared" si="14"/>
         <v>1942.4</v>
       </c>
-      <c r="I105" s="30"/>
-      <c r="J105" s="30"/>
-      <c r="K105" s="30"/>
+      <c r="I105" s="46"/>
+      <c r="J105" s="46"/>
+      <c r="K105" s="46"/>
     </row>
     <row r="106" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B106" s="16">
         <v>19</v>
       </c>
-      <c r="C106" s="42"/>
+      <c r="C106" s="43"/>
       <c r="D106" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E106" s="9">
         <v>25.5</v>
@@ -14587,17 +15413,17 @@
         <f t="shared" si="14"/>
         <v>1637.1</v>
       </c>
-      <c r="I106" s="30"/>
-      <c r="J106" s="30"/>
-      <c r="K106" s="30"/>
+      <c r="I106" s="46"/>
+      <c r="J106" s="46"/>
+      <c r="K106" s="46"/>
     </row>
     <row r="107" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B107" s="16">
         <v>20</v>
       </c>
-      <c r="C107" s="42"/>
+      <c r="C107" s="43"/>
       <c r="D107" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E107" s="9">
         <v>45</v>
@@ -14612,17 +15438,17 @@
         <f t="shared" si="14"/>
         <v>1597.2</v>
       </c>
-      <c r="I107" s="30"/>
-      <c r="J107" s="30"/>
-      <c r="K107" s="30"/>
+      <c r="I107" s="46"/>
+      <c r="J107" s="46"/>
+      <c r="K107" s="46"/>
     </row>
     <row r="108" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B108" s="16">
         <v>21</v>
       </c>
-      <c r="C108" s="42"/>
+      <c r="C108" s="43"/>
       <c r="D108" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E108" s="9">
         <v>75</v>
@@ -14637,19 +15463,19 @@
         <f t="shared" si="14"/>
         <v>1284</v>
       </c>
-      <c r="I108" s="30"/>
-      <c r="J108" s="30"/>
-      <c r="K108" s="30"/>
+      <c r="I108" s="46"/>
+      <c r="J108" s="46"/>
+      <c r="K108" s="46"/>
     </row>
     <row r="109" spans="2:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="16">
         <v>22</v>
       </c>
-      <c r="C109" s="39" t="s">
-        <v>41</v>
+      <c r="C109" s="61" t="s">
+        <v>40</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E109" s="11">
         <v>53</v>
@@ -14664,17 +15490,17 @@
       <c r="H109" s="11">
         <v>2500</v>
       </c>
-      <c r="I109" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="J109" s="38"/>
-      <c r="K109" s="38"/>
+      <c r="I109" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="J109" s="53"/>
+      <c r="K109" s="53"/>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B110" s="16">
         <v>23</v>
       </c>
-      <c r="C110" s="39"/>
+      <c r="C110" s="61"/>
       <c r="D110" s="11">
         <v>250</v>
       </c>
@@ -14691,15 +15517,15 @@
         <f t="shared" ref="H110:H120" si="15">ROUND(9550*F110/G110,1)</f>
         <v>1900.5</v>
       </c>
-      <c r="I110" s="38"/>
-      <c r="J110" s="38"/>
-      <c r="K110" s="38"/>
+      <c r="I110" s="53"/>
+      <c r="J110" s="53"/>
+      <c r="K110" s="53"/>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B111" s="16">
         <v>24</v>
       </c>
-      <c r="C111" s="39"/>
+      <c r="C111" s="61"/>
       <c r="D111" s="11">
         <v>500</v>
       </c>
@@ -14716,19 +15542,19 @@
         <f t="shared" si="15"/>
         <v>1900.5</v>
       </c>
-      <c r="I111" s="38"/>
-      <c r="J111" s="38"/>
-      <c r="K111" s="38"/>
+      <c r="I111" s="53"/>
+      <c r="J111" s="53"/>
+      <c r="K111" s="53"/>
     </row>
     <row r="112" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="16">
         <v>25</v>
       </c>
-      <c r="C112" s="28" t="s">
-        <v>92</v>
+      <c r="C112" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E112" s="4">
         <v>5.25</v>
@@ -14743,19 +15569,19 @@
         <f t="shared" si="15"/>
         <v>2319.3000000000002</v>
       </c>
-      <c r="I112" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="J112" s="43"/>
-      <c r="K112" s="43"/>
+      <c r="I112" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="J112" s="62"/>
+      <c r="K112" s="62"/>
     </row>
     <row r="113" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B113" s="16">
         <v>26</v>
       </c>
-      <c r="C113" s="28"/>
+      <c r="C113" s="27"/>
       <c r="D113" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E113" s="4">
         <v>7.5</v>
@@ -14770,17 +15596,17 @@
         <f t="shared" si="15"/>
         <v>2387.5</v>
       </c>
-      <c r="I113" s="43"/>
-      <c r="J113" s="43"/>
-      <c r="K113" s="43"/>
+      <c r="I113" s="62"/>
+      <c r="J113" s="62"/>
+      <c r="K113" s="62"/>
     </row>
     <row r="114" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B114" s="16">
         <v>27</v>
       </c>
-      <c r="C114" s="28"/>
+      <c r="C114" s="27"/>
       <c r="D114" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E114" s="4">
         <v>8</v>
@@ -14795,17 +15621,17 @@
         <f t="shared" si="15"/>
         <v>1989.6</v>
       </c>
-      <c r="I114" s="43"/>
-      <c r="J114" s="43"/>
-      <c r="K114" s="43"/>
+      <c r="I114" s="62"/>
+      <c r="J114" s="62"/>
+      <c r="K114" s="62"/>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B115" s="16">
         <v>28</v>
       </c>
-      <c r="C115" s="28"/>
+      <c r="C115" s="27"/>
       <c r="D115" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E115" s="4">
         <v>8.15</v>
@@ -14820,17 +15646,17 @@
         <f t="shared" si="15"/>
         <v>1910</v>
       </c>
-      <c r="I115" s="43"/>
-      <c r="J115" s="43"/>
-      <c r="K115" s="43"/>
+      <c r="I115" s="62"/>
+      <c r="J115" s="62"/>
+      <c r="K115" s="62"/>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B116" s="16">
         <v>29</v>
       </c>
-      <c r="C116" s="28"/>
+      <c r="C116" s="27"/>
       <c r="D116" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E116" s="4">
         <v>12</v>
@@ -14845,17 +15671,17 @@
         <f t="shared" si="15"/>
         <v>1910</v>
       </c>
-      <c r="I116" s="43"/>
-      <c r="J116" s="43"/>
-      <c r="K116" s="43"/>
+      <c r="I116" s="62"/>
+      <c r="J116" s="62"/>
+      <c r="K116" s="62"/>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B117" s="16">
         <v>30</v>
       </c>
-      <c r="C117" s="28"/>
+      <c r="C117" s="27"/>
       <c r="D117" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E117" s="4">
         <v>15.3</v>
@@ -14870,17 +15696,17 @@
         <f t="shared" si="15"/>
         <v>1719</v>
       </c>
-      <c r="I117" s="43"/>
-      <c r="J117" s="43"/>
-      <c r="K117" s="43"/>
+      <c r="I117" s="62"/>
+      <c r="J117" s="62"/>
+      <c r="K117" s="62"/>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B118" s="16">
         <v>31</v>
       </c>
-      <c r="C118" s="28"/>
+      <c r="C118" s="27"/>
       <c r="D118" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E118" s="4">
         <v>17.3</v>
@@ -14895,17 +15721,17 @@
         <f t="shared" si="15"/>
         <v>2387.5</v>
       </c>
-      <c r="I118" s="43"/>
-      <c r="J118" s="43"/>
-      <c r="K118" s="43"/>
+      <c r="I118" s="62"/>
+      <c r="J118" s="62"/>
+      <c r="K118" s="62"/>
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B119" s="16">
         <v>32</v>
       </c>
-      <c r="C119" s="29"/>
+      <c r="C119" s="28"/>
       <c r="D119" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E119" s="4">
         <v>23.8</v>
@@ -14920,16 +15746,16 @@
         <f t="shared" si="15"/>
         <v>2228.3000000000002</v>
       </c>
-      <c r="I119" s="43"/>
-      <c r="J119" s="43"/>
-      <c r="K119" s="43"/>
+      <c r="I119" s="62"/>
+      <c r="J119" s="62"/>
+      <c r="K119" s="62"/>
     </row>
     <row r="120" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="16">
         <v>33</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D120" s="3">
         <v>12030</v>
@@ -14947,21 +15773,21 @@
         <f t="shared" si="15"/>
         <v>#N/A</v>
       </c>
-      <c r="I120" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="J120" s="40"/>
-      <c r="K120" s="40"/>
+      <c r="I120" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="J120" s="44"/>
+      <c r="K120" s="44"/>
     </row>
     <row r="121" spans="2:11" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="16">
         <v>34</v>
       </c>
       <c r="C121" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D121" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="E121" s="8">
         <v>18</v>
@@ -14976,21 +15802,21 @@
       <c r="H121" s="8">
         <v>2500</v>
       </c>
-      <c r="I121" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="J121" s="41"/>
-      <c r="K121" s="41"/>
+      <c r="I121" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="J121" s="45"/>
+      <c r="K121" s="45"/>
     </row>
     <row r="122" spans="2:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="16">
         <v>35</v>
       </c>
-      <c r="C122" s="42" t="s">
-        <v>51</v>
+      <c r="C122" s="43" t="s">
+        <v>50</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E122" s="9">
         <v>13</v>
@@ -15005,19 +15831,19 @@
       <c r="H122" s="9">
         <v>2500</v>
       </c>
-      <c r="I122" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="J122" s="30"/>
-      <c r="K122" s="30"/>
+      <c r="I122" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="J122" s="46"/>
+      <c r="K122" s="46"/>
     </row>
     <row r="123" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B123" s="16">
         <v>36</v>
       </c>
-      <c r="C123" s="42"/>
+      <c r="C123" s="43"/>
       <c r="D123" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E123" s="9">
         <v>50</v>
@@ -15031,33 +15857,40 @@
       <c r="H123" s="9">
         <v>2500</v>
       </c>
-      <c r="I123" s="30"/>
-      <c r="J123" s="30"/>
-      <c r="K123" s="30"/>
+      <c r="I123" s="46"/>
+      <c r="J123" s="46"/>
+      <c r="K123" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="L45:L55"/>
-    <mergeCell ref="C45:C55"/>
-    <mergeCell ref="C88:C90"/>
-    <mergeCell ref="I86:K87"/>
-    <mergeCell ref="B83:K84"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="I120:K120"/>
-    <mergeCell ref="I121:K121"/>
-    <mergeCell ref="I122:K123"/>
-    <mergeCell ref="I99:K100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="L56:L60"/>
-    <mergeCell ref="L61:L63"/>
-    <mergeCell ref="L73:L78"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="L65:L66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="C56:C60"/>
-    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="L34:L41"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="C15:C24"/>
+    <mergeCell ref="L15:L24"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="L42:L44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="L27:L31"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="L10:L14"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="C91:C95"/>
     <mergeCell ref="I101:K101"/>
     <mergeCell ref="I102:K102"/>
@@ -15074,40 +15907,33 @@
     <mergeCell ref="H86:H87"/>
     <mergeCell ref="C96:C98"/>
     <mergeCell ref="I96:K98"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="I120:K120"/>
+    <mergeCell ref="I121:K121"/>
+    <mergeCell ref="I122:K123"/>
+    <mergeCell ref="I99:K100"/>
+    <mergeCell ref="C99:C100"/>
     <mergeCell ref="C109:C111"/>
     <mergeCell ref="C112:C119"/>
     <mergeCell ref="C103:C108"/>
     <mergeCell ref="I103:K108"/>
     <mergeCell ref="I109:K111"/>
     <mergeCell ref="I112:K119"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="L27:L31"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="L10:L14"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="L34:L41"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="C15:C24"/>
-    <mergeCell ref="L15:L24"/>
+    <mergeCell ref="L45:L55"/>
+    <mergeCell ref="C45:C55"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="I86:K87"/>
+    <mergeCell ref="B83:K84"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="L56:L60"/>
+    <mergeCell ref="L61:L63"/>
+    <mergeCell ref="L73:L78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="L65:L66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="C56:C60"/>
+    <mergeCell ref="C70:C72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>